<commit_message>
HR1 new version. Upload.
</commit_message>
<xml_diff>
--- a/data/HR1/Market Data/HR1_market_data_2020.xlsx
+++ b/data/HR1/Market Data/HR1_market_data_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\HR1\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B099D62-E6F8-435B-9573-A2BDC84BB1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74DDB9F-359E-48DE-88F6-A9EC9A85B7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27630" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -159,34 +159,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="B2">
-            <v>43.71</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="B2">
-            <v>48.115416666666654</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="B2">
-            <v>37.270000000000003</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="B2">
-            <v>37.574999999999996</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1373,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,10 +1363,11 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1">
-        <v>1</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D1" s="1">
         <f>1/3</f>
@@ -2792,7 +2769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B038B75F-C023-45BB-9C5E-2448F504CF83}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>